<commit_message>
experiment data && paper first draft
</commit_message>
<xml_diff>
--- a/note.xlsx
+++ b/note.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="rule" sheetId="1" r:id="rId1"/>
@@ -14,12 +14,11 @@
     <sheet name="exp-4" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="54">
   <si>
     <t>:</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,35 +160,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>null</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>exp-3：link失效的研究</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>benchmark</t>
+    <t>MRR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>link group size：1</t>
+    <t>precision_k</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>link group size：2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>precision</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>recall</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>f-measure</t>
+    <t>KDD'14</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -197,7 +180,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>KDD'14</t>
+    <t>size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>loss rate = 0.1%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>k=3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ToR crash 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ToR crash 2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#server crash</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检测时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询正确率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>犯错率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ToR crash 3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alpha = 0.6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alpha = 0.9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alpha = 0.4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -205,7 +240,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +317,14 @@
     </font>
     <font>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -389,7 +432,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -404,7 +447,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -414,9 +456,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2800,10 +2857,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AD57"/>
+  <dimension ref="A1:AD66"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -2837,21 +2894,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="30.6" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="G1" s="24" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="G1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
@@ -2859,39 +2916,39 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="20" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="2"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="21" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="20" t="s">
         <v>18</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="2"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="21" t="s">
+      <c r="L4" s="19"/>
+      <c r="M4" s="20" t="s">
         <v>23</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" s="2"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="21" t="s">
+      <c r="Q4" s="19"/>
+      <c r="R4" s="20" t="s">
         <v>24</v>
       </c>
       <c r="S4" s="1"/>
       <c r="T4" s="2"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="21" t="s">
+      <c r="V4" s="19"/>
+      <c r="W4" s="20" t="s">
         <v>25</v>
       </c>
       <c r="X4" s="1"/>
       <c r="Y4" s="2"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="21" t="s">
+      <c r="AA4" s="19"/>
+      <c r="AB4" s="20" t="s">
         <v>30</v>
       </c>
       <c r="AC4" s="1"/>
@@ -2910,7 +2967,7 @@
       <c r="D5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="17" t="s">
+      <c r="E5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -2922,7 +2979,7 @@
       <c r="I5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="17" t="s">
+      <c r="J5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="9" t="s">
@@ -2934,7 +2991,7 @@
       <c r="N5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O5" s="17" t="s">
+      <c r="O5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="Q5" s="9" t="s">
@@ -2946,7 +3003,7 @@
       <c r="S5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="T5" s="17" t="s">
+      <c r="T5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="V5" s="9" t="s">
@@ -2958,7 +3015,7 @@
       <c r="X5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="Y5" s="17" t="s">
+      <c r="Y5" s="16" t="s">
         <v>21</v>
       </c>
       <c r="AA5" s="9" t="s">
@@ -2970,7 +3027,7 @@
       <c r="AC5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AD5" s="17" t="s">
+      <c r="AD5" s="16" t="s">
         <v>21</v>
       </c>
     </row>
@@ -2992,7 +3049,7 @@
       <c r="H6" s="4">
         <v>0.99883599999999995</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="21">
         <v>0</v>
       </c>
       <c r="J6" s="8">
@@ -3045,7 +3102,7 @@
       <c r="H7" s="4">
         <v>0.97847600000000001</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="21">
         <v>0</v>
       </c>
       <c r="J7" s="8">
@@ -3098,7 +3155,7 @@
       <c r="H8" s="4">
         <v>0.95904500000000004</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="21">
         <v>0</v>
       </c>
       <c r="J8" s="8">
@@ -3151,7 +3208,7 @@
       <c r="H9" s="4">
         <v>0.93057699999999999</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="21">
         <v>0</v>
       </c>
       <c r="J9" s="8">
@@ -3204,7 +3261,7 @@
       <c r="H10" s="4">
         <v>0.93167800000000001</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="21">
         <v>0</v>
       </c>
       <c r="J10" s="8">
@@ -3261,7 +3318,7 @@
       <c r="H11" s="4">
         <v>0.89035500000000001</v>
       </c>
-      <c r="I11" s="22">
+      <c r="I11" s="21">
         <v>0</v>
       </c>
       <c r="J11" s="8">
@@ -3314,7 +3371,7 @@
       <c r="H12" s="4">
         <v>0.85354399999999997</v>
       </c>
-      <c r="I12" s="22">
+      <c r="I12" s="21">
         <v>0</v>
       </c>
       <c r="J12" s="8">
@@ -3375,7 +3432,7 @@
       <c r="H13" s="4">
         <v>0.82360199999999995</v>
       </c>
-      <c r="I13" s="22">
+      <c r="I13" s="21">
         <v>0</v>
       </c>
       <c r="J13" s="8">
@@ -3432,7 +3489,7 @@
       <c r="H14" s="4">
         <v>0.80350299999999997</v>
       </c>
-      <c r="I14" s="22">
+      <c r="I14" s="21">
         <v>0</v>
       </c>
       <c r="J14" s="8">
@@ -3493,7 +3550,7 @@
       <c r="H15" s="4">
         <v>0.80879000000000001</v>
       </c>
-      <c r="I15" s="22">
+      <c r="I15" s="21">
         <v>0</v>
       </c>
       <c r="J15" s="8">
@@ -3552,7 +3609,7 @@
       <c r="H16" s="4">
         <v>0.74650300000000003</v>
       </c>
-      <c r="I16" s="22">
+      <c r="I16" s="21">
         <v>0</v>
       </c>
       <c r="J16" s="8">
@@ -3613,7 +3670,7 @@
       <c r="H17" s="4">
         <v>0.69231900000000002</v>
       </c>
-      <c r="I17" s="22">
+      <c r="I17" s="21">
         <v>0</v>
       </c>
       <c r="J17" s="8">
@@ -3656,13 +3713,13 @@
       <c r="A18" s="5">
         <v>60</v>
       </c>
-      <c r="B18" s="18">
+      <c r="B18" s="17">
         <v>5</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="17">
         <v>0.75777000000000005</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="17">
         <v>0</v>
       </c>
       <c r="E18" s="11">
@@ -3671,42 +3728,42 @@
       <c r="G18" s="5">
         <v>17</v>
       </c>
-      <c r="H18" s="18">
+      <c r="H18" s="17">
         <v>0.708403</v>
       </c>
-      <c r="I18" s="18">
+      <c r="I18" s="17">
         <v>0</v>
       </c>
       <c r="J18" s="11">
         <v>0.31598999999999999</v>
       </c>
       <c r="L18" s="5"/>
-      <c r="M18" s="18"/>
-      <c r="N18" s="18"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
       <c r="O18" s="11"/>
       <c r="Q18" s="5">
         <v>9</v>
       </c>
-      <c r="R18" s="18">
+      <c r="R18" s="17">
         <v>0.733738</v>
       </c>
-      <c r="S18" s="18">
+      <c r="S18" s="17">
         <v>0</v>
       </c>
       <c r="T18" s="11">
         <v>0.34735199999999999</v>
       </c>
       <c r="V18" s="5"/>
-      <c r="W18" s="18"/>
-      <c r="X18" s="18"/>
+      <c r="W18" s="17"/>
+      <c r="X18" s="17"/>
       <c r="Y18" s="11"/>
       <c r="AA18" s="5">
         <v>30</v>
       </c>
-      <c r="AB18" s="18">
+      <c r="AB18" s="17">
         <v>0.55135599999999996</v>
       </c>
-      <c r="AC18" s="18">
+      <c r="AC18" s="17">
         <v>0</v>
       </c>
       <c r="AD18" s="11">
@@ -3727,23 +3784,23 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="2"/>
-      <c r="G23" s="20"/>
+      <c r="G23" s="19"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="2"/>
-      <c r="L23" s="20"/>
+      <c r="L23" s="19"/>
       <c r="M23" s="1"/>
       <c r="N23" s="1"/>
       <c r="O23" s="2"/>
-      <c r="Q23" s="20"/>
+      <c r="Q23" s="19"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="2"/>
-      <c r="V23" s="20"/>
+      <c r="V23" s="19"/>
       <c r="W23" s="1"/>
       <c r="X23" s="1"/>
       <c r="Y23" s="2"/>
-      <c r="AA23" s="20"/>
+      <c r="AA23" s="19"/>
       <c r="AB23" s="1"/>
       <c r="AC23" s="1"/>
       <c r="AD23" s="2"/>
@@ -3981,7 +4038,7 @@
       <c r="C29" s="4">
         <v>0.76277300000000003</v>
       </c>
-      <c r="D29" s="22">
+      <c r="D29" s="21">
         <v>447.5</v>
       </c>
       <c r="E29" s="8"/>
@@ -4290,22 +4347,22 @@
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
-        <v>0.05</v>
+        <v>1.2E-2</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4">
-        <v>3.8412000000000002E-2</v>
+        <v>0.33462999999999998</v>
       </c>
       <c r="D36" s="4">
-        <v>56.724138000000004</v>
+        <v>615.10344799999996</v>
       </c>
       <c r="E36" s="8"/>
       <c r="G36" s="3"/>
       <c r="H36" s="4">
-        <v>6.5089999999999995E-2</v>
+        <v>0.56123900000000004</v>
       </c>
       <c r="I36" s="4">
-        <v>101.34482800000001</v>
+        <v>754.63793099999998</v>
       </c>
       <c r="J36" s="8"/>
       <c r="L36" s="3"/>
@@ -4314,10 +4371,10 @@
       <c r="O36" s="8"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="4">
-        <v>5.5330999999999998E-2</v>
+        <v>0.57517799999999997</v>
       </c>
       <c r="S36" s="4">
-        <v>80.586207000000002</v>
+        <v>817.58620699999994</v>
       </c>
       <c r="T36" s="8"/>
       <c r="V36" s="3"/>
@@ -4326,822 +4383,1287 @@
       <c r="Y36" s="8"/>
       <c r="AA36" s="3"/>
       <c r="AB36" s="4">
-        <v>8.9538000000000006E-2</v>
+        <v>0.55361499999999997</v>
       </c>
       <c r="AC36" s="4">
-        <v>148.60344799999999</v>
+        <v>565.327586</v>
       </c>
       <c r="AD36" s="8"/>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A37" s="23">
-        <v>0.1</v>
-      </c>
-      <c r="B37" s="18"/>
-      <c r="C37" s="18">
-        <v>2.1953E-2</v>
-      </c>
-      <c r="D37" s="18">
-        <v>25.172414</v>
-      </c>
-      <c r="E37" s="11"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="18">
-        <v>3.2108999999999999E-2</v>
-      </c>
-      <c r="I37" s="18">
-        <v>32.879309999999997</v>
-      </c>
-      <c r="J37" s="11"/>
-      <c r="L37" s="5"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="11"/>
-      <c r="Q37" s="5"/>
-      <c r="R37" s="18">
-        <v>3.0093000000000002E-2</v>
-      </c>
-      <c r="S37" s="18">
-        <v>33.896552</v>
-      </c>
-      <c r="T37" s="11"/>
-      <c r="V37" s="5"/>
-      <c r="W37" s="18"/>
-      <c r="X37" s="18"/>
-      <c r="Y37" s="11"/>
-      <c r="AA37" s="5"/>
-      <c r="AB37" s="18">
-        <v>3.3987999999999997E-2</v>
-      </c>
-      <c r="AC37" s="18">
-        <v>42.275861999999996</v>
-      </c>
-      <c r="AD37" s="11"/>
+      <c r="A37" s="9">
+        <v>1.4E-2</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4">
+        <v>0.287192</v>
+      </c>
+      <c r="D37" s="4">
+        <v>549.84482800000001</v>
+      </c>
+      <c r="E37" s="8"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="4">
+        <v>0.50003600000000004</v>
+      </c>
+      <c r="I37" s="4">
+        <v>719.75862099999995</v>
+      </c>
+      <c r="J37" s="8"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="8"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="4">
+        <v>0.48594999999999999</v>
+      </c>
+      <c r="S37" s="4">
+        <v>869.60344799999996</v>
+      </c>
+      <c r="T37" s="8"/>
+      <c r="V37" s="3"/>
+      <c r="W37" s="4"/>
+      <c r="X37" s="4"/>
+      <c r="Y37" s="8"/>
+      <c r="AA37" s="3"/>
+      <c r="AB37" s="4">
+        <v>0.51798200000000005</v>
+      </c>
+      <c r="AC37" s="4">
+        <v>534.12068999999997</v>
+      </c>
+      <c r="AD37" s="8"/>
+    </row>
+    <row r="38" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>1.6E-2</v>
+      </c>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4">
+        <v>0.238179</v>
+      </c>
+      <c r="D38" s="4">
+        <v>491.84482000000003</v>
+      </c>
+      <c r="E38" s="8"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="4">
+        <v>0.42429600000000001</v>
+      </c>
+      <c r="I38" s="4">
+        <v>714.46551699999998</v>
+      </c>
+      <c r="J38" s="8"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="8"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="4">
+        <v>0.417966</v>
+      </c>
+      <c r="S38" s="4">
+        <v>824.43103399999995</v>
+      </c>
+      <c r="T38" s="8"/>
+      <c r="V38" s="3"/>
+      <c r="W38" s="4"/>
+      <c r="X38" s="4"/>
+      <c r="Y38" s="8"/>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="4">
+        <v>0.45116699999999998</v>
+      </c>
+      <c r="AC38" s="4">
+        <v>552.53448300000002</v>
+      </c>
+      <c r="AD38" s="8"/>
+    </row>
+    <row r="39" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4">
+        <v>0.20238500000000001</v>
+      </c>
+      <c r="D39" s="4">
+        <v>435.62069000000002</v>
+      </c>
+      <c r="E39" s="8"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="4">
+        <v>0.366367</v>
+      </c>
+      <c r="I39" s="4">
+        <v>692.29310299999997</v>
+      </c>
+      <c r="J39" s="8"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="8"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="4">
+        <v>0.35342699999999999</v>
+      </c>
+      <c r="S39" s="4">
+        <v>776.34482800000001</v>
+      </c>
+      <c r="T39" s="8"/>
+      <c r="V39" s="3"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="8"/>
+      <c r="AA39" s="3"/>
+      <c r="AB39" s="4">
+        <v>0.41221000000000002</v>
+      </c>
+      <c r="AC39" s="4">
+        <v>541.43103399999995</v>
+      </c>
+      <c r="AD39" s="8"/>
+    </row>
+    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>0.02</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="4">
+        <v>0.171316</v>
+      </c>
+      <c r="D40" s="4">
+        <v>384.39655199999999</v>
+      </c>
+      <c r="E40" s="8"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="4">
+        <v>0.325104</v>
+      </c>
+      <c r="I40" s="4">
+        <v>634.98275899999999</v>
+      </c>
+      <c r="J40" s="8"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="8"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="4">
+        <v>0.29713600000000001</v>
+      </c>
+      <c r="S40" s="4">
+        <v>690.36206900000002</v>
+      </c>
+      <c r="T40" s="8"/>
+      <c r="V40" s="3"/>
+      <c r="W40" s="4"/>
+      <c r="X40" s="4"/>
+      <c r="Y40" s="8"/>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="4">
+        <v>0.36954100000000001</v>
+      </c>
+      <c r="AC40" s="4">
+        <v>511.34482800000001</v>
+      </c>
+      <c r="AD40" s="8"/>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
-        <v>34</v>
-      </c>
+      <c r="A41" s="9">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4">
+        <v>0.12503</v>
+      </c>
+      <c r="D41" s="4">
+        <v>276.81034499999998</v>
+      </c>
+      <c r="E41" s="8"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="4">
+        <v>0.22126599999999999</v>
+      </c>
+      <c r="I41" s="4">
+        <v>485.77586200000002</v>
+      </c>
+      <c r="J41" s="8"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="8"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="4">
+        <v>0.19575699999999999</v>
+      </c>
+      <c r="S41" s="4">
+        <v>495.89655199999999</v>
+      </c>
+      <c r="T41" s="8"/>
+      <c r="V41" s="3"/>
+      <c r="W41" s="4"/>
+      <c r="X41" s="4"/>
+      <c r="Y41" s="8"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="4">
+        <v>0.29505300000000001</v>
+      </c>
+      <c r="AC41" s="4">
+        <v>430.81034499999998</v>
+      </c>
+      <c r="AD41" s="8"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A42" s="20"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="1"/>
-      <c r="E42" s="2"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="I42" s="1"/>
-      <c r="J42" s="2"/>
-      <c r="L42" s="20"/>
-      <c r="M42" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="N42" s="1"/>
-      <c r="O42" s="2"/>
-      <c r="Q42" s="20"/>
-      <c r="R42" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="S42" s="1"/>
-      <c r="T42" s="2"/>
-    </row>
-    <row r="43" spans="1:30" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="I43" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J43" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="L43" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="M43" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="N43" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O43" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q43" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R43" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="S43" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="T43" s="17" t="s">
-        <v>21</v>
-      </c>
+      <c r="A42" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="4">
+        <v>8.4197999999999995E-2</v>
+      </c>
+      <c r="D42" s="4">
+        <v>175.36206899999999</v>
+      </c>
+      <c r="E42" s="8"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="4">
+        <v>0.159251</v>
+      </c>
+      <c r="I42" s="4">
+        <v>344.86206900000002</v>
+      </c>
+      <c r="J42" s="8"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="8"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="4">
+        <v>0.13250999999999999</v>
+      </c>
+      <c r="S42" s="4">
+        <v>318.55172399999998</v>
+      </c>
+      <c r="T42" s="8"/>
+      <c r="V42" s="3"/>
+      <c r="W42" s="4"/>
+      <c r="X42" s="4"/>
+      <c r="Y42" s="8"/>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="4">
+        <v>0.22301499999999999</v>
+      </c>
+      <c r="AC42" s="4">
+        <v>361.29310299999997</v>
+      </c>
+      <c r="AD42" s="8"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="B43" s="4"/>
+      <c r="C43" s="4">
+        <v>6.4699000000000007E-2</v>
+      </c>
+      <c r="D43" s="4">
+        <v>127.189655</v>
+      </c>
+      <c r="E43" s="8"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="4">
+        <v>0.114879</v>
+      </c>
+      <c r="I43" s="4">
+        <v>243.22413800000001</v>
+      </c>
+      <c r="J43" s="8"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="8"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="4">
+        <v>9.7397999999999998E-2</v>
+      </c>
+      <c r="S43" s="4">
+        <v>201.53448299999999</v>
+      </c>
+      <c r="T43" s="8"/>
+      <c r="V43" s="3"/>
+      <c r="W43" s="4"/>
+      <c r="X43" s="4"/>
+      <c r="Y43" s="8"/>
+      <c r="AA43" s="3"/>
+      <c r="AB43" s="4">
+        <v>0.17838399999999999</v>
+      </c>
+      <c r="AC43" s="4">
+        <v>302.20689700000003</v>
+      </c>
+      <c r="AD43" s="8"/>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
-        <v>0</v>
+      <c r="A44" s="9">
+        <v>0.04</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4">
-        <v>0.91330500000000003</v>
+        <v>5.5551000000000003E-2</v>
       </c>
       <c r="D44" s="4">
-        <v>188.18966</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>96.034482999999994</v>
+      </c>
+      <c r="E44" s="8"/>
       <c r="G44" s="3"/>
       <c r="H44" s="4">
-        <v>0.990421</v>
+        <v>9.0719999999999995E-2</v>
       </c>
       <c r="I44" s="4">
-        <v>29.586207000000002</v>
-      </c>
-      <c r="J44" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>174.18965499999999</v>
+      </c>
+      <c r="J44" s="8"/>
       <c r="L44" s="3"/>
-      <c r="M44" s="4">
-        <v>0.99774499999999999</v>
-      </c>
-      <c r="N44" s="4">
-        <v>8.2068969999999997</v>
-      </c>
-      <c r="O44" s="8" t="s">
-        <v>35</v>
-      </c>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="8"/>
       <c r="Q44" s="3"/>
       <c r="R44" s="4">
-        <v>0.96091599999999999</v>
+        <v>7.1960999999999997E-2</v>
       </c>
       <c r="S44" s="4">
-        <v>91.465517000000006</v>
-      </c>
-      <c r="T44" s="8" t="s">
-        <v>35</v>
-      </c>
+        <v>132.586207</v>
+      </c>
+      <c r="T44" s="8"/>
+      <c r="V44" s="3"/>
+      <c r="W44" s="4"/>
+      <c r="X44" s="4"/>
+      <c r="Y44" s="8"/>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="4">
+        <v>0.13594500000000001</v>
+      </c>
+      <c r="AC44" s="4">
+        <v>234.36206899999999</v>
+      </c>
+      <c r="AD44" s="8"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
-        <v>1</v>
+      <c r="A45" s="9">
+        <v>0.05</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4">
-        <v>0.91172299999999995</v>
+        <v>3.8412000000000002E-2</v>
       </c>
       <c r="D45" s="4">
-        <v>199.413793</v>
-      </c>
-      <c r="E45" s="8">
-        <v>0.20887700000000001</v>
-      </c>
+        <v>56.724138000000004</v>
+      </c>
+      <c r="E45" s="8"/>
       <c r="G45" s="3"/>
       <c r="H45" s="4">
-        <v>0.99194099999999996</v>
-      </c>
-      <c r="I45" s="22">
-        <v>24.482759000000001</v>
-      </c>
-      <c r="J45" s="8">
-        <v>0.20887700000000001</v>
-      </c>
+        <v>6.5089999999999995E-2</v>
+      </c>
+      <c r="I45" s="4">
+        <v>101.34482800000001</v>
+      </c>
+      <c r="J45" s="8"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="4">
-        <v>0.99786799999999998</v>
-      </c>
-      <c r="N45" s="4">
-        <v>3.9827590000000002</v>
-      </c>
-      <c r="O45" s="8">
-        <v>0.20887700000000001</v>
-      </c>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="8"/>
       <c r="Q45" s="3"/>
       <c r="R45" s="4">
-        <v>0.95863900000000002</v>
+        <v>5.5330999999999998E-2</v>
       </c>
       <c r="S45" s="4">
-        <v>90.603448</v>
-      </c>
-      <c r="T45" s="8">
-        <v>0.108977</v>
-      </c>
+        <v>80.586207000000002</v>
+      </c>
+      <c r="T45" s="8"/>
+      <c r="V45" s="3"/>
+      <c r="W45" s="4"/>
+      <c r="X45" s="4"/>
+      <c r="Y45" s="8"/>
+      <c r="AA45" s="3"/>
+      <c r="AB45" s="4">
+        <v>8.9538000000000006E-2</v>
+      </c>
+      <c r="AC45" s="4">
+        <v>148.60344799999999</v>
+      </c>
+      <c r="AD45" s="8"/>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
-        <v>5</v>
-      </c>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4">
-        <v>0.90050399999999997</v>
-      </c>
-      <c r="D46" s="4">
-        <v>174.172414</v>
-      </c>
-      <c r="E46" s="8">
-        <v>0.23624999999999999</v>
-      </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="4">
-        <v>0.97212600000000005</v>
-      </c>
-      <c r="I46" s="22">
-        <v>25</v>
-      </c>
-      <c r="J46" s="8">
-        <v>0.19678999999999999</v>
-      </c>
-      <c r="L46" s="3"/>
-      <c r="M46" s="4">
-        <v>0.97641</v>
-      </c>
-      <c r="N46" s="4">
-        <v>10.413793</v>
-      </c>
-      <c r="O46" s="8">
-        <v>0.25624999999999998</v>
-      </c>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="4">
-        <v>0.93756300000000004</v>
-      </c>
-      <c r="S46" s="4">
-        <v>101.706897</v>
-      </c>
-      <c r="T46" s="8">
-        <v>0.23629</v>
-      </c>
-    </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
-        <v>10</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4">
-        <v>0.88682399999999995</v>
-      </c>
-      <c r="D47" s="4">
-        <v>166.37931</v>
-      </c>
-      <c r="E47" s="8">
-        <v>0.235987</v>
-      </c>
-      <c r="G47" s="3"/>
-      <c r="H47" s="4">
-        <v>0.951542</v>
-      </c>
-      <c r="I47" s="22">
-        <v>22.068966</v>
-      </c>
-      <c r="J47" s="8">
-        <v>0.31600699999999998</v>
-      </c>
-      <c r="L47" s="3"/>
-      <c r="M47" s="4">
-        <v>0.957874</v>
-      </c>
-      <c r="N47" s="4">
-        <v>7.0517240000000001</v>
-      </c>
-      <c r="O47" s="8">
-        <v>0.25598700000000002</v>
-      </c>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="4">
-        <v>0.92678199999999999</v>
-      </c>
-      <c r="S47" s="4">
-        <v>72.827585999999997</v>
-      </c>
-      <c r="T47" s="8">
-        <v>0.25605699999999998</v>
-      </c>
-    </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>15</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4">
-        <v>0.86403300000000005</v>
-      </c>
-      <c r="D48" s="4">
-        <v>176.89655200000001</v>
-      </c>
-      <c r="E48" s="8">
-        <v>0.23411599999999999</v>
-      </c>
-      <c r="G48" s="3"/>
-      <c r="H48" s="4">
-        <v>0.92286400000000002</v>
-      </c>
-      <c r="I48" s="22">
-        <v>25.448276</v>
-      </c>
-      <c r="J48" s="8">
-        <v>0.28105599999999997</v>
-      </c>
-      <c r="L48" s="3"/>
-      <c r="M48" s="4">
-        <v>0.93190700000000004</v>
-      </c>
-      <c r="N48" s="4">
-        <v>6.0344829999999998</v>
-      </c>
-      <c r="O48" s="8">
-        <v>0.24771599999999999</v>
-      </c>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="4">
-        <v>0.89111499999999999</v>
-      </c>
-      <c r="S48" s="4">
-        <v>85.706896999999998</v>
-      </c>
-      <c r="T48" s="8">
-        <v>0.24043200000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+      <c r="A46" s="22">
+        <v>0.1</v>
+      </c>
+      <c r="B46" s="17"/>
+      <c r="C46" s="17">
+        <v>2.1953E-2</v>
+      </c>
+      <c r="D46" s="17">
+        <v>25.172414</v>
+      </c>
+      <c r="E46" s="11"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="17">
+        <v>3.2108999999999999E-2</v>
+      </c>
+      <c r="I46" s="17">
+        <v>32.879309999999997</v>
+      </c>
+      <c r="J46" s="11"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="11"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="17">
+        <v>3.0093000000000002E-2</v>
+      </c>
+      <c r="S46" s="17">
+        <v>33.896552</v>
+      </c>
+      <c r="T46" s="11"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="17"/>
+      <c r="X46" s="17"/>
+      <c r="Y46" s="11"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="17">
+        <v>3.3987999999999997E-2</v>
+      </c>
+      <c r="AC46" s="17">
+        <v>42.275861999999996</v>
+      </c>
+      <c r="AD46" s="11"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A50" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="2"/>
+      <c r="G51" s="19"/>
+      <c r="H51" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="2"/>
+      <c r="L51" s="19"/>
+      <c r="M51" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="N51" s="1"/>
+      <c r="O51" s="2"/>
+      <c r="Q51" s="19"/>
+      <c r="R51" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="S51" s="1"/>
+      <c r="T51" s="2"/>
+    </row>
+    <row r="52" spans="1:20" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4">
-        <v>0.870641</v>
-      </c>
-      <c r="D49" s="4">
-        <v>141.172414</v>
-      </c>
-      <c r="E49" s="8">
-        <v>0.226187</v>
-      </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="4">
-        <v>0.92616200000000004</v>
-      </c>
-      <c r="I49" s="22">
-        <v>19.534483000000002</v>
-      </c>
-      <c r="J49" s="8">
-        <v>0.23517299999999999</v>
-      </c>
-      <c r="L49" s="3"/>
-      <c r="M49" s="4">
-        <v>0.93144000000000005</v>
-      </c>
-      <c r="N49" s="4">
-        <v>2.3448280000000001</v>
-      </c>
-      <c r="O49" s="8">
-        <v>0.22689300000000001</v>
-      </c>
-      <c r="Q49" s="3">
-        <v>2</v>
-      </c>
-      <c r="R49" s="4">
-        <v>0.88188200000000005</v>
-      </c>
-      <c r="S49" s="4">
-        <v>69.931033999999997</v>
-      </c>
-      <c r="T49" s="8">
-        <v>0.21598200000000001</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
-        <v>25</v>
-      </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4">
-        <v>0.84576799999999996</v>
-      </c>
-      <c r="D50" s="4">
-        <v>120.4482756</v>
-      </c>
-      <c r="E50" s="8">
-        <v>0.22262299999999999</v>
-      </c>
-      <c r="G50" s="3">
-        <v>1</v>
-      </c>
-      <c r="H50" s="4">
-        <v>0.88769900000000002</v>
-      </c>
-      <c r="I50" s="22">
-        <v>12.465517</v>
-      </c>
-      <c r="J50" s="8">
-        <v>0.33472000000000002</v>
-      </c>
-      <c r="L50" s="3"/>
-      <c r="M50" s="4">
-        <v>0.89018399999999998</v>
-      </c>
-      <c r="N50" s="4">
-        <v>5.9310340000000004</v>
-      </c>
-      <c r="O50" s="8">
-        <v>0.266067</v>
-      </c>
-      <c r="Q50" s="3">
-        <v>1</v>
-      </c>
-      <c r="R50" s="4">
-        <v>0.86239500000000002</v>
-      </c>
-      <c r="S50" s="4">
-        <v>75.982759000000001</v>
-      </c>
-      <c r="T50" s="8">
-        <v>0.24690000000000001</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
-        <v>30</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4">
-        <v>0.81239099999999997</v>
-      </c>
-      <c r="D51" s="4">
-        <v>131.25862100000001</v>
-      </c>
-      <c r="E51" s="8">
-        <v>0.17644699999999999</v>
-      </c>
-      <c r="G51" s="3"/>
-      <c r="H51" s="4">
-        <v>0.85126100000000005</v>
-      </c>
-      <c r="I51" s="22">
-        <v>14.706897</v>
-      </c>
-      <c r="J51" s="8">
-        <v>0.30625200000000002</v>
-      </c>
-      <c r="L51" s="3">
-        <v>2</v>
-      </c>
-      <c r="M51" s="4">
-        <v>0.85523300000000002</v>
-      </c>
-      <c r="N51" s="4">
-        <v>3.4310339999999999</v>
-      </c>
-      <c r="O51" s="8">
-        <v>0.22914499999999999</v>
-      </c>
-      <c r="Q51" s="3">
-        <v>4</v>
-      </c>
-      <c r="R51" s="4">
-        <v>0.80108000000000001</v>
-      </c>
-      <c r="S51" s="4">
-        <v>56.206896999999998</v>
-      </c>
-      <c r="T51" s="8">
-        <v>0.236427</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="3">
-        <v>35</v>
-      </c>
-      <c r="B52" s="4">
-        <v>1</v>
-      </c>
-      <c r="C52" s="4">
-        <v>0.79000099999999995</v>
-      </c>
-      <c r="D52" s="4">
-        <v>120.224138</v>
-      </c>
-      <c r="E52" s="8">
-        <v>0.23966899999999999</v>
-      </c>
-      <c r="G52" s="3">
-        <v>1</v>
-      </c>
-      <c r="H52" s="4">
-        <v>0.82142499999999996</v>
-      </c>
-      <c r="I52" s="22">
-        <v>13.5</v>
-      </c>
-      <c r="J52" s="8">
-        <v>0.30947799999999998</v>
-      </c>
-      <c r="L52" s="3"/>
-      <c r="M52" s="4">
-        <v>0.83758600000000005</v>
-      </c>
-      <c r="N52" s="4">
-        <v>1.4137930000000001</v>
-      </c>
-      <c r="O52" s="8">
-        <v>0.2913</v>
-      </c>
-      <c r="Q52" s="3">
-        <v>7</v>
-      </c>
-      <c r="R52" s="4">
-        <v>0.79827199999999998</v>
-      </c>
-      <c r="S52" s="4">
-        <v>56.241379000000002</v>
-      </c>
-      <c r="T52" s="8">
-        <v>0.19567300000000001</v>
+      <c r="E52" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G52" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J52" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="L52" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="M52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N52" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O52" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q52" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="R52" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="S52" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="T52" s="16" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>40</v>
-      </c>
-      <c r="B53" s="4"/>
+        <v>0</v>
+      </c>
+      <c r="B53" s="4">
+        <v>0</v>
+      </c>
       <c r="C53" s="4">
-        <v>0.76736099999999996</v>
+        <v>0.91330500000000003</v>
       </c>
       <c r="D53" s="4">
-        <v>123.94827600000001</v>
+        <v>188.18966</v>
       </c>
       <c r="E53" s="8">
-        <v>0.213614</v>
+        <v>0</v>
       </c>
       <c r="G53" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H53" s="4">
-        <v>0.80106999999999995</v>
-      </c>
-      <c r="I53" s="22">
-        <v>12.12069</v>
+        <v>0.990421</v>
+      </c>
+      <c r="I53" s="4">
+        <v>29.586207000000002</v>
       </c>
       <c r="J53" s="8">
-        <v>0.27613799999999999</v>
+        <v>0</v>
       </c>
       <c r="L53" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="M53" s="4">
-        <v>0.80699100000000001</v>
+        <v>0.99774499999999999</v>
       </c>
       <c r="N53" s="4">
-        <v>1.362069</v>
+        <v>8.2068969999999997</v>
       </c>
       <c r="O53" s="8">
-        <v>0.30546699999999999</v>
+        <v>0</v>
       </c>
       <c r="Q53" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="R53" s="4">
-        <v>0.78861400000000004</v>
-      </c>
-      <c r="S53" s="22">
-        <v>69.5</v>
+        <v>0.96091599999999999</v>
+      </c>
+      <c r="S53" s="4">
+        <v>91.465517000000006</v>
       </c>
       <c r="T53" s="8">
-        <v>0.22082299999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>45</v>
+        <v>1</v>
       </c>
       <c r="B54" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C54" s="4">
-        <v>0.79499399999999998</v>
+        <v>0.91172299999999995</v>
       </c>
       <c r="D54" s="4">
-        <v>84.086207000000002</v>
+        <v>199.413793</v>
       </c>
       <c r="E54" s="8">
-        <v>0.26604</v>
+        <v>0.20887700000000001</v>
       </c>
       <c r="G54" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H54" s="4">
-        <v>0.80636200000000002</v>
-      </c>
-      <c r="I54" s="22">
-        <v>10.172414</v>
+        <v>0.99194099999999996</v>
+      </c>
+      <c r="I54" s="21">
+        <v>24.482759000000001</v>
       </c>
       <c r="J54" s="8">
-        <v>0.33344800000000002</v>
+        <v>0.20887700000000001</v>
       </c>
       <c r="L54" s="3">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="M54" s="4">
-        <v>0.79092799999999996</v>
+        <v>0.99786799999999998</v>
       </c>
       <c r="N54" s="4">
-        <v>2.0172409999999998</v>
+        <v>3.9827590000000002</v>
       </c>
       <c r="O54" s="8">
-        <v>0.27222400000000002</v>
+        <v>0.20887700000000001</v>
       </c>
       <c r="Q54" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R54" s="4">
-        <v>0.76230699999999996</v>
+        <v>0.95863900000000002</v>
       </c>
       <c r="S54" s="4">
-        <v>44.655172</v>
+        <v>90.603448</v>
       </c>
       <c r="T54" s="8">
-        <v>0.23180300000000001</v>
+        <v>0.108977</v>
       </c>
     </row>
     <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>50</v>
-      </c>
-      <c r="B55" s="4"/>
+        <v>5</v>
+      </c>
+      <c r="B55" s="4">
+        <v>0</v>
+      </c>
       <c r="C55" s="4">
-        <v>0.73388900000000001</v>
+        <v>0.90050399999999997</v>
       </c>
       <c r="D55" s="4">
-        <v>97.982759000000001</v>
+        <v>174.172414</v>
       </c>
       <c r="E55" s="8">
-        <v>0.263351</v>
+        <v>0.23624999999999999</v>
       </c>
       <c r="G55" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="H55" s="4">
-        <v>0.74534400000000001</v>
-      </c>
-      <c r="I55" s="22">
-        <v>8.1206899999999997</v>
+        <v>0.97212600000000005</v>
+      </c>
+      <c r="I55" s="21">
+        <v>25</v>
       </c>
       <c r="J55" s="8">
-        <v>0.32631199999999999</v>
+        <v>0.19678999999999999</v>
       </c>
       <c r="L55" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="M55" s="4">
-        <v>0.74543700000000002</v>
+        <v>0.97641</v>
       </c>
       <c r="N55" s="4">
-        <v>0.68965500000000002</v>
+        <v>10.413793</v>
       </c>
       <c r="O55" s="8">
-        <v>0.29361799999999999</v>
+        <v>0.25624999999999998</v>
       </c>
       <c r="Q55" s="3">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="R55" s="4">
-        <v>0.68177900000000002</v>
+        <v>0.93756300000000004</v>
       </c>
       <c r="S55" s="4">
-        <v>48.827585999999997</v>
+        <v>101.706897</v>
       </c>
       <c r="T55" s="8">
-        <v>0.26205299999999998</v>
+        <v>0.23629</v>
       </c>
     </row>
     <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
+        <v>10</v>
+      </c>
+      <c r="B56" s="4">
+        <v>0</v>
+      </c>
+      <c r="C56" s="4">
+        <v>0.88682399999999995</v>
+      </c>
+      <c r="D56" s="4">
+        <v>166.37931</v>
+      </c>
+      <c r="E56" s="8">
+        <v>0.235987</v>
+      </c>
+      <c r="G56" s="3">
+        <v>0</v>
+      </c>
+      <c r="H56" s="4">
+        <v>0.951542</v>
+      </c>
+      <c r="I56" s="21">
+        <v>22.068966</v>
+      </c>
+      <c r="J56" s="8">
+        <v>0.31600699999999998</v>
+      </c>
+      <c r="L56" s="3">
+        <v>0</v>
+      </c>
+      <c r="M56" s="4">
+        <v>0.957874</v>
+      </c>
+      <c r="N56" s="4">
+        <v>7.0517240000000001</v>
+      </c>
+      <c r="O56" s="8">
+        <v>0.25598700000000002</v>
+      </c>
+      <c r="Q56" s="3">
+        <v>0</v>
+      </c>
+      <c r="R56" s="4">
+        <v>0.92678199999999999</v>
+      </c>
+      <c r="S56" s="4">
+        <v>72.827585999999997</v>
+      </c>
+      <c r="T56" s="8">
+        <v>0.25605699999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>15</v>
+      </c>
+      <c r="B57" s="4">
+        <v>0</v>
+      </c>
+      <c r="C57" s="4">
+        <v>0.86403300000000005</v>
+      </c>
+      <c r="D57" s="4">
+        <v>176.89655200000001</v>
+      </c>
+      <c r="E57" s="8">
+        <v>0.23411599999999999</v>
+      </c>
+      <c r="G57" s="3">
+        <v>0</v>
+      </c>
+      <c r="H57" s="4">
+        <v>0.92286400000000002</v>
+      </c>
+      <c r="I57" s="21">
+        <v>25.448276</v>
+      </c>
+      <c r="J57" s="8">
+        <v>0.28105599999999997</v>
+      </c>
+      <c r="L57" s="3">
+        <v>0</v>
+      </c>
+      <c r="M57" s="4">
+        <v>0.93190700000000004</v>
+      </c>
+      <c r="N57" s="4">
+        <v>6.0344829999999998</v>
+      </c>
+      <c r="O57" s="8">
+        <v>0.24771599999999999</v>
+      </c>
+      <c r="Q57" s="3">
+        <v>0</v>
+      </c>
+      <c r="R57" s="4">
+        <v>0.89111499999999999</v>
+      </c>
+      <c r="S57" s="4">
+        <v>85.706896999999998</v>
+      </c>
+      <c r="T57" s="8">
+        <v>0.24043200000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>20</v>
+      </c>
+      <c r="B58" s="4">
+        <v>0</v>
+      </c>
+      <c r="C58" s="4">
+        <v>0.870641</v>
+      </c>
+      <c r="D58" s="4">
+        <v>141.172414</v>
+      </c>
+      <c r="E58" s="8">
+        <v>0.226187</v>
+      </c>
+      <c r="G58" s="3">
+        <v>0</v>
+      </c>
+      <c r="H58" s="4">
+        <v>0.92616200000000004</v>
+      </c>
+      <c r="I58" s="21">
+        <v>19.534483000000002</v>
+      </c>
+      <c r="J58" s="8">
+        <v>0.23517299999999999</v>
+      </c>
+      <c r="L58" s="3">
+        <v>0</v>
+      </c>
+      <c r="M58" s="4">
+        <v>0.93144000000000005</v>
+      </c>
+      <c r="N58" s="4">
+        <v>2.3448280000000001</v>
+      </c>
+      <c r="O58" s="8">
+        <v>0.22689300000000001</v>
+      </c>
+      <c r="Q58" s="3">
+        <v>2</v>
+      </c>
+      <c r="R58" s="4">
+        <v>0.88188200000000005</v>
+      </c>
+      <c r="S58" s="4">
+        <v>69.931033999999997</v>
+      </c>
+      <c r="T58" s="8">
+        <v>0.21598200000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>25</v>
+      </c>
+      <c r="B59" s="4">
+        <v>0</v>
+      </c>
+      <c r="C59" s="4">
+        <v>0.84576799999999996</v>
+      </c>
+      <c r="D59" s="4">
+        <v>120.4482756</v>
+      </c>
+      <c r="E59" s="8">
+        <v>0.22262299999999999</v>
+      </c>
+      <c r="G59" s="3">
+        <v>1</v>
+      </c>
+      <c r="H59" s="4">
+        <v>0.88769900000000002</v>
+      </c>
+      <c r="I59" s="21">
+        <v>12.465517</v>
+      </c>
+      <c r="J59" s="8">
+        <v>0.33472000000000002</v>
+      </c>
+      <c r="L59" s="3">
+        <v>0</v>
+      </c>
+      <c r="M59" s="4">
+        <v>0.89018399999999998</v>
+      </c>
+      <c r="N59" s="4">
+        <v>5.9310340000000004</v>
+      </c>
+      <c r="O59" s="8">
+        <v>0.266067</v>
+      </c>
+      <c r="Q59" s="3">
+        <v>1</v>
+      </c>
+      <c r="R59" s="4">
+        <v>0.86239500000000002</v>
+      </c>
+      <c r="S59" s="4">
+        <v>75.982759000000001</v>
+      </c>
+      <c r="T59" s="8">
+        <v>0.24690000000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>30</v>
+      </c>
+      <c r="B60" s="4">
+        <v>0</v>
+      </c>
+      <c r="C60" s="4">
+        <v>0.81239099999999997</v>
+      </c>
+      <c r="D60" s="4">
+        <v>131.25862100000001</v>
+      </c>
+      <c r="E60" s="8">
+        <v>0.17644699999999999</v>
+      </c>
+      <c r="G60" s="3">
+        <v>0</v>
+      </c>
+      <c r="H60" s="4">
+        <v>0.85126100000000005</v>
+      </c>
+      <c r="I60" s="21">
+        <v>14.706897</v>
+      </c>
+      <c r="J60" s="8">
+        <v>0.30625200000000002</v>
+      </c>
+      <c r="L60" s="3">
+        <v>2</v>
+      </c>
+      <c r="M60" s="4">
+        <v>0.85523300000000002</v>
+      </c>
+      <c r="N60" s="4">
+        <v>3.4310339999999999</v>
+      </c>
+      <c r="O60" s="8">
+        <v>0.22914499999999999</v>
+      </c>
+      <c r="Q60" s="3">
+        <v>4</v>
+      </c>
+      <c r="R60" s="4">
+        <v>0.80108000000000001</v>
+      </c>
+      <c r="S60" s="4">
+        <v>56.206896999999998</v>
+      </c>
+      <c r="T60" s="8">
+        <v>0.236427</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>35</v>
+      </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
+      <c r="C61" s="4">
+        <v>0.79000099999999995</v>
+      </c>
+      <c r="D61" s="4">
+        <v>120.224138</v>
+      </c>
+      <c r="E61" s="8">
+        <v>0.23966899999999999</v>
+      </c>
+      <c r="G61" s="3">
+        <v>1</v>
+      </c>
+      <c r="H61" s="4">
+        <v>0.82142499999999996</v>
+      </c>
+      <c r="I61" s="21">
+        <v>13.5</v>
+      </c>
+      <c r="J61" s="8">
+        <v>0.30947799999999998</v>
+      </c>
+      <c r="L61" s="3">
+        <v>0</v>
+      </c>
+      <c r="M61" s="4">
+        <v>0.83758600000000005</v>
+      </c>
+      <c r="N61" s="4">
+        <v>1.4137930000000001</v>
+      </c>
+      <c r="O61" s="8">
+        <v>0.2913</v>
+      </c>
+      <c r="Q61" s="3">
+        <v>7</v>
+      </c>
+      <c r="R61" s="4">
+        <v>0.79827199999999998</v>
+      </c>
+      <c r="S61" s="4">
+        <v>56.241379000000002</v>
+      </c>
+      <c r="T61" s="8">
+        <v>0.19567300000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>40</v>
+      </c>
+      <c r="B62" s="21">
+        <v>0</v>
+      </c>
+      <c r="C62" s="4">
+        <v>0.76736099999999996</v>
+      </c>
+      <c r="D62" s="4">
+        <v>123.94827600000001</v>
+      </c>
+      <c r="E62" s="8">
+        <v>0.213614</v>
+      </c>
+      <c r="G62" s="3">
+        <v>2</v>
+      </c>
+      <c r="H62" s="4">
+        <v>0.80106999999999995</v>
+      </c>
+      <c r="I62" s="21">
+        <v>12.12069</v>
+      </c>
+      <c r="J62" s="8">
+        <v>0.27613799999999999</v>
+      </c>
+      <c r="L62" s="3">
+        <v>2</v>
+      </c>
+      <c r="M62" s="4">
+        <v>0.80699100000000001</v>
+      </c>
+      <c r="N62" s="4">
+        <v>1.362069</v>
+      </c>
+      <c r="O62" s="8">
+        <v>0.30546699999999999</v>
+      </c>
+      <c r="Q62" s="3">
+        <v>5</v>
+      </c>
+      <c r="R62" s="4">
+        <v>0.78861400000000004</v>
+      </c>
+      <c r="S62" s="21">
+        <v>69.5</v>
+      </c>
+      <c r="T62" s="8">
+        <v>0.22082299999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>45</v>
+      </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
+      <c r="C63" s="4">
+        <v>0.79499399999999998</v>
+      </c>
+      <c r="D63" s="4">
+        <v>84.086207000000002</v>
+      </c>
+      <c r="E63" s="8">
+        <v>0.26604</v>
+      </c>
+      <c r="G63" s="3">
+        <v>5</v>
+      </c>
+      <c r="H63" s="4">
+        <v>0.80636200000000002</v>
+      </c>
+      <c r="I63" s="21">
+        <v>10.172414</v>
+      </c>
+      <c r="J63" s="8">
+        <v>0.33344800000000002</v>
+      </c>
+      <c r="L63" s="3">
+        <v>4</v>
+      </c>
+      <c r="M63" s="4">
+        <v>0.79092799999999996</v>
+      </c>
+      <c r="N63" s="4">
+        <v>2.0172409999999998</v>
+      </c>
+      <c r="O63" s="8">
+        <v>0.27222400000000002</v>
+      </c>
+      <c r="Q63" s="3">
+        <v>1</v>
+      </c>
+      <c r="R63" s="4">
+        <v>0.76230699999999996</v>
+      </c>
+      <c r="S63" s="4">
+        <v>44.655172</v>
+      </c>
+      <c r="T63" s="8">
+        <v>0.23180300000000001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>50</v>
+      </c>
+      <c r="B64" s="21">
+        <v>0</v>
+      </c>
+      <c r="C64" s="4">
+        <v>0.73388900000000001</v>
+      </c>
+      <c r="D64" s="4">
+        <v>97.982759000000001</v>
+      </c>
+      <c r="E64" s="8">
+        <v>0.263351</v>
+      </c>
+      <c r="G64" s="3">
+        <v>6</v>
+      </c>
+      <c r="H64" s="4">
+        <v>0.74534400000000001</v>
+      </c>
+      <c r="I64" s="21">
+        <v>8.1206899999999997</v>
+      </c>
+      <c r="J64" s="8">
+        <v>0.32631199999999999</v>
+      </c>
+      <c r="L64" s="3">
+        <v>7</v>
+      </c>
+      <c r="M64" s="4">
+        <v>0.74543700000000002</v>
+      </c>
+      <c r="N64" s="4">
+        <v>0.68965500000000002</v>
+      </c>
+      <c r="O64" s="8">
+        <v>0.29361799999999999</v>
+      </c>
+      <c r="Q64" s="3">
+        <v>7</v>
+      </c>
+      <c r="R64" s="4">
+        <v>0.68177900000000002</v>
+      </c>
+      <c r="S64" s="4">
+        <v>48.827585999999997</v>
+      </c>
+      <c r="T64" s="8">
+        <v>0.26205299999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
         <v>55</v>
       </c>
-      <c r="B56" s="4">
+      <c r="B65" s="4">
         <v>4</v>
       </c>
-      <c r="C56" s="4">
+      <c r="C65" s="4">
         <v>0.68861000000000006</v>
       </c>
-      <c r="D56" s="4">
+      <c r="D65" s="4">
         <v>107.103448</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E65" s="8">
         <v>0.22345799999999999</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G65" s="3">
         <v>9</v>
       </c>
-      <c r="H56" s="4">
+      <c r="H65" s="4">
         <v>0.69058399999999998</v>
       </c>
-      <c r="I56" s="22">
+      <c r="I65" s="21">
         <v>8.1551720000000003</v>
       </c>
-      <c r="J56" s="8">
+      <c r="J65" s="8">
         <v>0.32612400000000002</v>
       </c>
-      <c r="L56" s="3">
+      <c r="L65" s="3">
         <v>6</v>
       </c>
-      <c r="M56" s="4">
+      <c r="M65" s="4">
         <v>0.70238</v>
       </c>
-      <c r="N56" s="4">
+      <c r="N65" s="4">
         <v>1.5517240000000001</v>
       </c>
-      <c r="O56" s="8">
+      <c r="O65" s="8">
         <v>0.28081</v>
       </c>
-      <c r="Q56" s="3">
+      <c r="Q65" s="3">
         <v>20</v>
       </c>
-      <c r="R56" s="4">
+      <c r="R65" s="4">
         <v>0.71407799999999999</v>
       </c>
-      <c r="S56" s="4">
+      <c r="S65" s="4">
         <v>52.413792999999998</v>
       </c>
-      <c r="T56" s="8">
+      <c r="T65" s="8">
         <v>0.21911700000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A57" s="5">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A66" s="5">
         <v>60</v>
       </c>
-      <c r="B57" s="18">
+      <c r="B66" s="17">
         <v>5</v>
       </c>
-      <c r="C57" s="18">
+      <c r="C66" s="17">
         <v>0.73641800000000002</v>
       </c>
-      <c r="D57" s="18">
+      <c r="D66" s="17">
         <v>72.620689999999996</v>
       </c>
-      <c r="E57" s="11">
+      <c r="E66" s="11">
         <v>0.273424</v>
       </c>
-      <c r="G57" s="5">
+      <c r="G66" s="5">
         <v>17</v>
       </c>
-      <c r="H57" s="18">
+      <c r="H66" s="17">
         <v>0.70847899999999997</v>
       </c>
-      <c r="I57" s="18">
+      <c r="I66" s="17">
         <v>0.39655200000000002</v>
       </c>
-      <c r="J57" s="11">
+      <c r="J66" s="11">
         <v>0.29738500000000001</v>
       </c>
-      <c r="L57" s="5">
+      <c r="L66" s="5">
         <v>9</v>
       </c>
-      <c r="M57" s="18">
+      <c r="M66" s="17">
         <v>0.73377899999999996</v>
       </c>
-      <c r="N57" s="18">
-        <v>0</v>
-      </c>
-      <c r="O57" s="11">
+      <c r="N66" s="17">
+        <v>0</v>
+      </c>
+      <c r="O66" s="11">
         <v>0.34176800000000002</v>
       </c>
-      <c r="Q57" s="5">
+      <c r="Q66" s="5">
         <v>31</v>
       </c>
-      <c r="R57" s="18">
+      <c r="R66" s="17">
         <v>0.54417300000000002</v>
       </c>
-      <c r="S57" s="18">
+      <c r="S66" s="17">
         <v>13.241379</v>
       </c>
-      <c r="T57" s="11">
+      <c r="T66" s="11">
         <v>0.25476100000000002</v>
       </c>
     </row>
@@ -5174,10 +5696,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30.6" x14ac:dyDescent="0.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="16"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
@@ -5279,97 +5801,174 @@
   <sheetPr>
     <tabColor theme="9" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.6640625" customWidth="1"/>
-    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" ht="25.8" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="26"/>
+      <c r="B3" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="27"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="27"/>
+    </row>
+    <row r="4" spans="1:10" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+      <c r="D4" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C5" s="12" t="s">
+      <c r="I4" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
+    </row>
+    <row r="5" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="28">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="B5" s="29">
+        <v>0.8</v>
+      </c>
+      <c r="C5" s="29">
+        <v>0.86670000000000003</v>
+      </c>
+      <c r="D5" s="30">
+        <v>5.4977999999999998</v>
+      </c>
+      <c r="G5" s="28">
+        <v>1</v>
+      </c>
+      <c r="H5" s="34">
+        <v>1</v>
+      </c>
+      <c r="I5" s="34">
+        <v>1</v>
+      </c>
+      <c r="J5" s="30">
+        <v>0.1933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B6" s="29">
+        <v>0.3</v>
+      </c>
+      <c r="C6" s="29">
+        <v>0.7167</v>
+      </c>
+      <c r="D6" s="33">
+        <v>6.2112999999999996</v>
+      </c>
+      <c r="G6" s="28">
+        <v>2</v>
+      </c>
+      <c r="H6" s="34">
+        <v>1</v>
+      </c>
+      <c r="I6" s="34">
+        <v>1</v>
+      </c>
+      <c r="J6" s="30">
+        <v>1.0314000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="B7" s="29">
+        <v>0.66669999999999996</v>
+      </c>
+      <c r="C7" s="29">
+        <v>1</v>
+      </c>
+      <c r="D7" s="30">
+        <v>6.1604000000000001</v>
+      </c>
+      <c r="G7" s="28">
+        <v>3</v>
+      </c>
+      <c r="H7" s="29">
+        <v>0.73329999999999995</v>
+      </c>
+      <c r="I7" s="29">
+        <v>1</v>
+      </c>
+      <c r="J7" s="30">
+        <v>0.79749999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="35">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
-        <v>39</v>
-      </c>
-    </row>
+      <c r="B8" s="31">
+        <v>0.6</v>
+      </c>
+      <c r="C8" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="D8" s="32">
+        <v>6.2652000000000001</v>
+      </c>
+      <c r="G8" s="35">
+        <v>4</v>
+      </c>
+      <c r="H8" s="36">
+        <v>0.75</v>
+      </c>
+      <c r="I8" s="36">
+        <v>1</v>
+      </c>
+      <c r="J8" s="32">
+        <v>1.4277</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:10" s="25" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5378,24 +5977,399 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="22.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0.59581399999999995</v>
+      </c>
+      <c r="C8">
+        <v>0.98016899999999996</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0.59591400000000005</v>
+      </c>
+      <c r="C9">
+        <v>0.98016800000000004</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>0.59591400000000005</v>
+      </c>
+      <c r="C10">
+        <v>0.98016800000000004</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>0.59591400000000005</v>
+      </c>
+      <c r="C11">
+        <v>0.92923599999999995</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>40</v>
+      </c>
+      <c r="B12">
+        <v>0.59591400000000005</v>
+      </c>
+      <c r="C12">
+        <v>0.84379000000000004</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>50</v>
+      </c>
+      <c r="B13">
+        <v>0.59591400000000005</v>
+      </c>
+      <c r="C13">
+        <v>0.98016800000000004</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>60</v>
+      </c>
+      <c r="B14">
+        <v>0.59591400000000005</v>
+      </c>
+      <c r="C14">
+        <v>0.83496400000000004</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>0.523258</v>
+      </c>
+      <c r="C18">
+        <v>0.93303899999999995</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19">
+        <v>0.523258</v>
+      </c>
+      <c r="C19">
+        <v>0.93303800000000003</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>0.57325800000000005</v>
+      </c>
+      <c r="C20">
+        <v>0.932751</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>30</v>
+      </c>
+      <c r="B21">
+        <v>0.523258</v>
+      </c>
+      <c r="C21">
+        <v>0.93303899999999995</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>40</v>
+      </c>
+      <c r="B22">
+        <v>0.523258</v>
+      </c>
+      <c r="C22">
+        <v>0.78963899999999998</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>50</v>
+      </c>
+      <c r="B23">
+        <v>0.523258</v>
+      </c>
+      <c r="C23">
+        <v>0.77797499999999997</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>60</v>
+      </c>
+      <c r="B24">
+        <v>0.57325800000000005</v>
+      </c>
+      <c r="C24">
+        <v>0.90489699999999995</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="25">
+        <v>0</v>
+      </c>
+      <c r="B31" s="25">
+        <v>0.36987500000000001</v>
+      </c>
+      <c r="C31" s="25">
+        <v>0.74768999999999997</v>
+      </c>
+      <c r="D31" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32">
+        <v>0.40087499999999998</v>
+      </c>
+      <c r="C32">
+        <v>0.74742299999999995</v>
+      </c>
+      <c r="D32" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>0.40784199999999998</v>
+      </c>
+      <c r="C33">
+        <v>0.66015699999999999</v>
+      </c>
+      <c r="D33" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>0.40317500000000001</v>
+      </c>
+      <c r="C34">
+        <v>0.74143800000000004</v>
+      </c>
+      <c r="D34" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>0.40317500000000001</v>
+      </c>
+      <c r="C35">
+        <v>0.70379999999999998</v>
+      </c>
+      <c r="D35" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>50</v>
+      </c>
+      <c r="B36">
+        <v>0.43654199999999999</v>
+      </c>
+      <c r="C36">
+        <v>0.65351499999999996</v>
+      </c>
+      <c r="D36" s="25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>60</v>
+      </c>
+      <c r="B37">
+        <v>0.417265</v>
+      </c>
+      <c r="C37">
+        <v>0.64917000000000002</v>
+      </c>
+      <c r="D37" s="25">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>